<commit_message>
Set invoice address to payee's
</commit_message>
<xml_diff>
--- a/app/invoices/templates/invoice_template.xlsx
+++ b/app/invoices/templates/invoice_template.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t xml:space="preserve">COMMERCIAL INVOICE</t>
   </si>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">Kazarova Zhanna</t>
   </si>
   <si>
-    <t xml:space="preserve">Comapany Name</t>
+    <t xml:space="preserve">Company Name</t>
   </si>
   <si>
     <t xml:space="preserve">TALYAGLOBAL</t>
@@ -200,9 +200,6 @@
   </si>
   <si>
     <t xml:space="preserve">INV-2020-08-0017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Company Name</t>
   </si>
   <si>
     <t xml:space="preserve">83psc</t>
@@ -1391,7 +1388,7 @@
   <dimension ref="A3:E556"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.62109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3986,7 +3983,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="25" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>10</v>
@@ -6427,7 +6424,7 @@
       <c r="B311" s="65"/>
       <c r="C311" s="69"/>
       <c r="D311" s="70" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E311" s="71"/>
     </row>

</xml_diff>